<commit_message>
Added ROI Count Workflow
</commit_message>
<xml_diff>
--- a/Processed PO Numbers.xlsx
+++ b/Processed PO Numbers.xlsx
@@ -193,6 +193,72 @@
   </x:si>
   <x:si>
     <x:t>SO-00022135</x:t>
+  </x:si>
+  <x:si>
+    <x:t>101865(0120860)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SO-00022146</x:t>
+  </x:si>
+  <x:si>
+    <x:t>77218(0119760)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SO-00022147</x:t>
+  </x:si>
+  <x:si>
+    <x:t>421818(109260)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SO-00022151</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60317(0125160)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SO-00022152</x:t>
+  </x:si>
+  <x:si>
+    <x:t>308312(0104460)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SO-00022153</x:t>
+  </x:si>
+  <x:si>
+    <x:t>358566(0106160)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SO-00022154</x:t>
+  </x:si>
+  <x:si>
+    <x:t>499485(0102060)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SO-00022195</x:t>
+  </x:si>
+  <x:si>
+    <x:t>281788(0104060)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SO-00022196</x:t>
+  </x:si>
+  <x:si>
+    <x:t>449581(0102860)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SO-00022197</x:t>
+  </x:si>
+  <x:si>
+    <x:t>215931(0115960)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SO-00022206</x:t>
+  </x:si>
+  <x:si>
+    <x:t>434129(0107560)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SO-00022207</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -752,7 +818,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -763,7 +829,7 @@
         <x:v>44</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -774,7 +840,7 @@
         <x:v>46</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:3">
@@ -785,7 +851,7 @@
         <x:v>48</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:3">
@@ -796,7 +862,7 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:3">
@@ -807,7 +873,7 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:3">
@@ -818,6 +884,127 @@
         <x:v>54</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:3">
+      <x:c r="A27" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:3">
+      <x:c r="A28" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:3">
+      <x:c r="A29" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:3">
+      <x:c r="A30" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:3">
+      <x:c r="A31" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:3">
+      <x:c r="A32" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:3">
+      <x:c r="A33" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:3">
+      <x:c r="A34" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:3">
+      <x:c r="A35" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:3">
+      <x:c r="A36" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:3">
+      <x:c r="A37" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>

</xml_diff>